<commit_message>
updated creds in temp branch
</commit_message>
<xml_diff>
--- a/test-data/test_case_template.xlsx
+++ b/test-data/test_case_template.xlsx
@@ -64,7 +64,7 @@
     <t>Vishal</t>
   </si>
   <si>
-    <t>Password</t>
+    <t>Password56</t>
   </si>
 </sst>
 </file>
@@ -72,7 +72,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +105,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Inter"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -164,7 +170,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -211,6 +217,13 @@
       <bottom style="thin">
         <color rgb="FFffffff"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -302,77 +315,77 @@
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="7" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="8" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="7" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="8" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -874,7 +887,7 @@
       <c r="AB5" s="8"/>
       <c r="AC5" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="21.75">
       <c r="A6" s="9"/>
       <c r="B6" s="10"/>
       <c r="C6" s="11"/>
@@ -905,7 +918,7 @@
       <c r="AB6" s="8"/>
       <c r="AC6" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="21.75">
       <c r="A7" s="9"/>
       <c r="B7" s="10"/>
       <c r="C7" s="11"/>
@@ -936,7 +949,7 @@
       <c r="AB7" s="8"/>
       <c r="AC7" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="21.75">
       <c r="A8" s="1"/>
       <c r="B8" s="14"/>
       <c r="C8" s="15"/>
@@ -967,7 +980,7 @@
       <c r="AB8" s="8"/>
       <c r="AC8" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="21.75">
       <c r="A9" s="1"/>
       <c r="B9" s="16"/>
       <c r="C9" s="17"/>

</xml_diff>